<commit_message>
Remove envelope costs from BASoBC
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BASoBC/BAU Amt Spent on Bldg Components.xlsx
+++ b/InputData/bldgs/BASoBC/BAU Amt Spent on Bldg Components.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="170">
   <si>
     <t>BASoBC BAU Amount Spent on Building Components</t>
   </si>
@@ -557,6 +557,9 @@
   <si>
     <t>$</t>
   </si>
+  <si>
+    <t>The EPS does not handle changes in envelope costs.</t>
+  </si>
 </sst>
 </file>
 
@@ -1003,7 +1006,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1079,7 +1081,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="#,##0.0000000000" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2462,9 +2463,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -2734,6 +2737,11 @@
     <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove envelope costs from BASoBC xlsx file
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BASoBC/BAU Amt Spent on Bldg Components.xlsx
+++ b/InputData/bldgs/BASoBC/BAU Amt Spent on Bldg Components.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\bldgs\BASoBC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-india\InputData\bldgs\BASoBC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2764,8 +2764,8 @@
   </sheetPr>
   <dimension ref="A1:AL7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:AL4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3202,152 +3202,115 @@
         <v>13</v>
       </c>
       <c r="B4" s="6">
-        <f t="shared" si="0"/>
-        <v>10715659161.443731</v>
+        <v>0</v>
       </c>
       <c r="C4" s="6">
-        <f t="shared" si="1"/>
-        <v>10715659161.443731</v>
+        <v>0</v>
       </c>
       <c r="D4" s="6">
-        <f t="shared" si="1"/>
-        <v>10715659161.443731</v>
-      </c>
-      <c r="E4" s="9">
-        <f>'Calculations 2'!B54</f>
-        <v>10715659161.443731</v>
-      </c>
-      <c r="F4" s="9">
-        <f>'Calculations 2'!C54</f>
-        <v>11326161436.261013</v>
-      </c>
-      <c r="G4" s="9">
-        <f>'Calculations 2'!D54</f>
-        <v>11407010441.858749</v>
-      </c>
-      <c r="H4" s="9">
-        <f>'Calculations 2'!E54</f>
-        <v>11487859447.456543</v>
-      </c>
-      <c r="I4" s="9">
-        <f>'Calculations 2'!F54</f>
-        <v>11568708453.056213</v>
-      </c>
-      <c r="J4" s="9">
-        <f>'Calculations 2'!G54</f>
-        <v>11649557458.652225</v>
-      </c>
-      <c r="K4" s="9">
-        <f>'Calculations 2'!H54</f>
-        <v>10409819281.321047</v>
-      </c>
-      <c r="L4" s="9">
-        <f>'Calculations 2'!I54</f>
-        <v>10465183271.108898</v>
-      </c>
-      <c r="M4" s="9">
-        <f>'Calculations 2'!J54</f>
-        <v>10520547260.896711</v>
-      </c>
-      <c r="N4" s="9">
-        <f>'Calculations 2'!K54</f>
-        <v>10575911250.682663</v>
-      </c>
-      <c r="O4" s="9">
-        <f>'Calculations 2'!L54</f>
-        <v>10631275240.469624</v>
-      </c>
-      <c r="P4" s="9">
-        <f>'Calculations 2'!M54</f>
-        <v>11082249866.901928</v>
-      </c>
-      <c r="Q4" s="9">
-        <f>'Calculations 2'!N54</f>
-        <v>11145248447.920527</v>
-      </c>
-      <c r="R4" s="9">
-        <f>'Calculations 2'!O54</f>
-        <v>11208247028.940842</v>
-      </c>
-      <c r="S4" s="9">
-        <f>'Calculations 2'!P54</f>
-        <v>11271245609.961275</v>
-      </c>
-      <c r="T4" s="9">
-        <f>'Calculations 2'!Q54</f>
-        <v>11334244190.982561</v>
-      </c>
-      <c r="U4" s="9">
-        <f>'Calculations 2'!R54</f>
-        <v>9967189772.424593</v>
-      </c>
-      <c r="V4" s="9">
-        <f>'Calculations 2'!S54</f>
-        <v>10002590839.419001</v>
-      </c>
-      <c r="W4" s="9">
-        <f>'Calculations 2'!T54</f>
-        <v>10037991906.412886</v>
-      </c>
-      <c r="X4" s="9">
-        <f>'Calculations 2'!U54</f>
-        <v>10073392973.405933</v>
-      </c>
-      <c r="Y4" s="9">
-        <f>'Calculations 2'!V54</f>
-        <v>10108794040.399818</v>
-      </c>
-      <c r="Z4" s="9">
-        <f>'Calculations 2'!W54</f>
-        <v>10422492427.940308</v>
-      </c>
-      <c r="AA4" s="9">
-        <f>'Calculations 2'!X54</f>
-        <v>10463264144.978514</v>
-      </c>
-      <c r="AB4" s="9">
-        <f>'Calculations 2'!Y54</f>
-        <v>10504035862.018518</v>
-      </c>
-      <c r="AC4" s="9">
-        <f>'Calculations 2'!Z54</f>
-        <v>10544807579.056726</v>
-      </c>
-      <c r="AD4" s="9">
-        <f>'Calculations 2'!AA54</f>
-        <v>10585579296.096727</v>
-      </c>
-      <c r="AE4" s="9">
-        <f>'Calculations 2'!AB54</f>
-        <v>9178701156.3222847</v>
-      </c>
-      <c r="AF4" s="9">
-        <f>'Calculations 2'!AC54</f>
-        <v>9191535770.8617306</v>
-      </c>
-      <c r="AG4" s="9">
-        <f>'Calculations 2'!AD54</f>
-        <v>9204370385.4006977</v>
-      </c>
-      <c r="AH4" s="9">
-        <f>'Calculations 2'!AE54</f>
-        <v>9217204999.9400826</v>
-      </c>
-      <c r="AI4" s="9">
-        <f>'Calculations 2'!AF54</f>
-        <v>9230039614.4791088</v>
-      </c>
-      <c r="AJ4" s="9">
-        <f>'Calculations 2'!AG54</f>
-        <v>9242874229.0185528</v>
-      </c>
-      <c r="AK4" s="9">
-        <f>'Calculations 2'!AH54</f>
-        <v>9255708843.5577621</v>
-      </c>
-      <c r="AL4" s="9">
-        <f>'Calculations 2'!AI54</f>
-        <v>9268543458.0967274</v>
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0</v>
+      </c>
+      <c r="O4" s="6">
+        <v>0</v>
+      </c>
+      <c r="P4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>0</v>
+      </c>
+      <c r="R4" s="6">
+        <v>0</v>
+      </c>
+      <c r="S4" s="6">
+        <v>0</v>
+      </c>
+      <c r="T4" s="6">
+        <v>0</v>
+      </c>
+      <c r="U4" s="6">
+        <v>0</v>
+      </c>
+      <c r="V4" s="6">
+        <v>0</v>
+      </c>
+      <c r="W4" s="6">
+        <v>0</v>
+      </c>
+      <c r="X4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.45">
@@ -3821,8 +3784,8 @@
   </sheetPr>
   <dimension ref="A1:AL7"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:AL3"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:AL4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4258,152 +4221,115 @@
         <v>13</v>
       </c>
       <c r="B4" s="6">
-        <f t="shared" si="0"/>
-        <v>191085394.83042541</v>
+        <v>0</v>
       </c>
       <c r="C4" s="6">
-        <f t="shared" si="1"/>
-        <v>191085394.83042541</v>
+        <v>0</v>
       </c>
       <c r="D4" s="6">
-        <f t="shared" si="1"/>
-        <v>191085394.83042541</v>
-      </c>
-      <c r="E4" s="9">
-        <f>'Calculations 2'!B82</f>
-        <v>191085394.83042541</v>
-      </c>
-      <c r="F4" s="9">
-        <f>'Calculations 2'!C82</f>
-        <v>570728895.50225139</v>
-      </c>
-      <c r="G4" s="9">
-        <f>'Calculations 2'!D82</f>
-        <v>957731982.82981169</v>
-      </c>
-      <c r="H4" s="9">
-        <f>'Calculations 2'!E82</f>
-        <v>1352094656.6456592</v>
-      </c>
-      <c r="I4" s="9">
-        <f>'Calculations 2'!F82</f>
-        <v>1753816916.2564676</v>
-      </c>
-      <c r="J4" s="9">
-        <f>'Calculations 2'!G82</f>
-        <v>2162898762.5230122</v>
-      </c>
-      <c r="K4" s="9">
-        <f>'Calculations 2'!H82</f>
-        <v>2579340195.1036744</v>
-      </c>
-      <c r="L4" s="9">
-        <f>'Calculations 2'!I82</f>
-        <v>3003141213.9113607</v>
-      </c>
-      <c r="M4" s="9">
-        <f>'Calculations 2'!J82</f>
-        <v>3434301819.1185727</v>
-      </c>
-      <c r="N4" s="9">
-        <f>'Calculations 2'!K82</f>
-        <v>3872822010.4657278</v>
-      </c>
-      <c r="O4" s="9">
-        <f>'Calculations 2'!L82</f>
-        <v>4318701788.1236324</v>
-      </c>
-      <c r="P4" s="9">
-        <f>'Calculations 2'!M82</f>
-        <v>4771941152.4406395</v>
-      </c>
-      <c r="Q4" s="9">
-        <f>'Calculations 2'!N82</f>
-        <v>5232540102.726778</v>
-      </c>
-      <c r="R4" s="9">
-        <f>'Calculations 2'!O82</f>
-        <v>5700498639.4107466</v>
-      </c>
-      <c r="S4" s="9">
-        <f>'Calculations 2'!P82</f>
-        <v>6175816762.4071674</v>
-      </c>
-      <c r="T4" s="9">
-        <f>'Calculations 2'!Q82</f>
-        <v>6658494471.716013</v>
-      </c>
-      <c r="U4" s="9">
-        <f>'Calculations 2'!R82</f>
-        <v>7148531767.5114622</v>
-      </c>
-      <c r="V4" s="9">
-        <f>'Calculations 2'!S82</f>
-        <v>7645928649.4485483</v>
-      </c>
-      <c r="W4" s="9">
-        <f>'Calculations 2'!T82</f>
-        <v>8150685117.5238819</v>
-      </c>
-      <c r="X4" s="9">
-        <f>'Calculations 2'!U82</f>
-        <v>8662801172.430809</v>
-      </c>
-      <c r="Y4" s="9">
-        <f>'Calculations 2'!V82</f>
-        <v>9182276812.960207</v>
-      </c>
-      <c r="Z4" s="9">
-        <f>'Calculations 2'!W82</f>
-        <v>9709112040.3178291</v>
-      </c>
-      <c r="AA4" s="9">
-        <f>'Calculations 2'!X82</f>
-        <v>10243306853.991264</v>
-      </c>
-      <c r="AB4" s="9">
-        <f>'Calculations 2'!Y82</f>
-        <v>10784861253.806299</v>
-      </c>
-      <c r="AC4" s="9">
-        <f>'Calculations 2'!Z82</f>
-        <v>11333775239.585436</v>
-      </c>
-      <c r="AD4" s="9">
-        <f>'Calculations 2'!AA82</f>
-        <v>11890048812.36697</v>
-      </c>
-      <c r="AE4" s="9">
-        <f>'Calculations 2'!AB82</f>
-        <v>12453681971.119328</v>
-      </c>
-      <c r="AF4" s="9">
-        <f>'Calculations 2'!AC82</f>
-        <v>13024674715.835768</v>
-      </c>
-      <c r="AG4" s="9">
-        <f>'Calculations 2'!AD82</f>
-        <v>13603027047.728785</v>
-      </c>
-      <c r="AH4" s="9">
-        <f>'Calculations 2'!AE82</f>
-        <v>14188738965.247595</v>
-      </c>
-      <c r="AI4" s="9">
-        <f>'Calculations 2'!AF82</f>
-        <v>14781810469.075548</v>
-      </c>
-      <c r="AJ4" s="9">
-        <f>'Calculations 2'!AG82</f>
-        <v>15382241559.735016</v>
-      </c>
-      <c r="AK4" s="9">
-        <f>'Calculations 2'!AH82</f>
-        <v>15990032236.365362</v>
-      </c>
-      <c r="AL4" s="9">
-        <f>'Calculations 2'!AI82</f>
-        <v>16605182498.959753</v>
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0</v>
+      </c>
+      <c r="O4" s="6">
+        <v>0</v>
+      </c>
+      <c r="P4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>0</v>
+      </c>
+      <c r="R4" s="6">
+        <v>0</v>
+      </c>
+      <c r="S4" s="6">
+        <v>0</v>
+      </c>
+      <c r="T4" s="6">
+        <v>0</v>
+      </c>
+      <c r="U4" s="6">
+        <v>0</v>
+      </c>
+      <c r="V4" s="6">
+        <v>0</v>
+      </c>
+      <c r="W4" s="6">
+        <v>0</v>
+      </c>
+      <c r="X4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.45">
@@ -18109,8 +18035,8 @@
   </sheetPr>
   <dimension ref="A1:AL7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:AL4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -18547,152 +18473,115 @@
         <v>13</v>
       </c>
       <c r="B4" s="6">
-        <f t="shared" si="0"/>
-        <v>9688694120.3146515</v>
+        <v>0</v>
       </c>
       <c r="C4" s="6">
-        <f t="shared" si="1"/>
-        <v>9688694120.3146515</v>
+        <v>0</v>
       </c>
       <c r="D4" s="6">
-        <f t="shared" si="1"/>
-        <v>9688694120.3146515</v>
+        <v>0</v>
       </c>
       <c r="E4" s="6">
-        <f>'Calculations 2'!B26</f>
-        <v>9688694120.3146515</v>
+        <v>0</v>
       </c>
       <c r="F4" s="6">
-        <f>'Calculations 2'!C26</f>
-        <v>11046263268.022633</v>
+        <v>0</v>
       </c>
       <c r="G4" s="6">
-        <f>'Calculations 2'!D26</f>
-        <v>11191601556.120682</v>
+        <v>0</v>
       </c>
       <c r="H4" s="6">
-        <f>'Calculations 2'!E26</f>
-        <v>11336939844.218761</v>
+        <v>0</v>
       </c>
       <c r="I4" s="6">
-        <f>'Calculations 2'!F26</f>
-        <v>11482278132.31678</v>
+        <v>0</v>
       </c>
       <c r="J4" s="6">
-        <f>'Calculations 2'!G26</f>
-        <v>11627616420.412987</v>
+        <v>0</v>
       </c>
       <c r="K4" s="6">
-        <f>'Calculations 2'!H26</f>
-        <v>12081492179.399916</v>
+        <v>0</v>
       </c>
       <c r="L4" s="6">
-        <f>'Calculations 2'!I26</f>
-        <v>12232784699.390432</v>
+        <v>0</v>
       </c>
       <c r="M4" s="6">
-        <f>'Calculations 2'!J26</f>
-        <v>12384077219.380913</v>
+        <v>0</v>
       </c>
       <c r="N4" s="6">
-        <f>'Calculations 2'!K26</f>
-        <v>12535369739.375048</v>
+        <v>0</v>
       </c>
       <c r="O4" s="6">
-        <f>'Calculations 2'!L26</f>
-        <v>12686662259.365498</v>
+        <v>0</v>
       </c>
       <c r="P4" s="6">
-        <f>'Calculations 2'!M26</f>
-        <v>14232213991.858164</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="6">
-        <f>'Calculations 2'!N26</f>
-        <v>14410413268.584698</v>
+        <v>0</v>
       </c>
       <c r="R4" s="6">
-        <f>'Calculations 2'!O26</f>
-        <v>14588612545.305826</v>
+        <v>0</v>
       </c>
       <c r="S4" s="6">
-        <f>'Calculations 2'!P26</f>
-        <v>14766811822.030603</v>
+        <v>0</v>
       </c>
       <c r="T4" s="6">
-        <f>'Calculations 2'!Q26</f>
-        <v>14945011098.758945</v>
+        <v>0</v>
       </c>
       <c r="U4" s="6">
-        <f>'Calculations 2'!R26</f>
-        <v>15316632588.201284</v>
+        <v>0</v>
       </c>
       <c r="V4" s="6">
-        <f>'Calculations 2'!S26</f>
-        <v>15498564574.297993</v>
+        <v>0</v>
       </c>
       <c r="W4" s="6">
-        <f>'Calculations 2'!T26</f>
-        <v>15680496560.394772</v>
+        <v>0</v>
       </c>
       <c r="X4" s="6">
-        <f>'Calculations 2'!U26</f>
-        <v>15862428546.484306</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="6">
-        <f>'Calculations 2'!V26</f>
-        <v>16044360532.577337</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="6">
-        <f>'Calculations 2'!W26</f>
-        <v>17782621236.860752</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="6">
-        <f>'Calculations 2'!X26</f>
-        <v>17994587636.813656</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="6">
-        <f>'Calculations 2'!Y26</f>
-        <v>18206554036.76656</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="6">
-        <f>'Calculations 2'!Z26</f>
-        <v>18418520436.723152</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="6">
-        <f>'Calculations 2'!AA26</f>
-        <v>18630486836.672443</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="6">
-        <f>'Calculations 2'!AB26</f>
-        <v>18939360083.451763</v>
+        <v>0</v>
       </c>
       <c r="AF4" s="6">
-        <f>'Calculations 2'!AC26</f>
-        <v>19153196615.54015</v>
+        <v>0</v>
       </c>
       <c r="AG4" s="6">
-        <f>'Calculations 2'!AD26</f>
-        <v>19367033147.62112</v>
+        <v>0</v>
       </c>
       <c r="AH4" s="6">
-        <f>'Calculations 2'!AE26</f>
-        <v>19580869679.709507</v>
+        <v>0</v>
       </c>
       <c r="AI4" s="6">
-        <f>'Calculations 2'!AF26</f>
-        <v>19794706211.790478</v>
+        <v>0</v>
       </c>
       <c r="AJ4" s="6">
-        <f>'Calculations 2'!AG26</f>
-        <v>20008542743.878811</v>
+        <v>0</v>
       </c>
       <c r="AK4" s="6">
-        <f>'Calculations 2'!AH26</f>
-        <v>20222379275.963581</v>
+        <v>0</v>
       </c>
       <c r="AL4" s="6">
-        <f>'Calculations 2'!AI26</f>
-        <v>20436215808.044544</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.45">

</xml_diff>